<commit_message>
Inserting the operations treeview in the summary tab
- Inserting the operations treeview in the summary tab
- Adding some information in the operations dataframe:
   > market
   > duration in days and months
   > rentability
- Improving the PORTFOLIO_TEMPLATE.xlsx file
</commit_message>
<xml_diff>
--- a/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
+++ b/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dudu\Finanças\Investimentos\Mercado Financeiro\Investment_Portfolio_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dudu\Finanças\Investimentos\Mercado Financeiro\Investment_Portfolio_Analysis\portfolio_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Extrato" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$P$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$P$35</definedName>
     <definedName name="Aplica">#REF!</definedName>
     <definedName name="CDI">#REF!</definedName>
     <definedName name="IR0.0">#REF!</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="43">
   <si>
     <t>Data</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>BBAS3</t>
-  </si>
-  <si>
-    <t>Provento</t>
   </si>
   <si>
     <t>Cobrança</t>
@@ -567,13 +564,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,16 +620,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -658,7 +655,7 @@
         <v>1010</v>
       </c>
       <c r="J2" s="7">
-        <f t="shared" ref="J2:J9" si="0">H2*I2</f>
+        <f t="shared" ref="J2:J8" si="0">H2*I2</f>
         <v>1010</v>
       </c>
       <c r="K2" s="7">
@@ -674,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="7">
-        <f t="shared" ref="O2:O9" si="1">K2+L2</f>
+        <f t="shared" ref="O2:O8" si="1">K2+L2</f>
         <v>10</v>
       </c>
       <c r="P2" s="4"/>
@@ -728,10 +725,10 @@
         <v>41971</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="4">
         <v>49444</v>
@@ -787,7 +784,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -819,82 +816,82 @@
     </row>
     <row r="6" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>42045</v>
+        <v>42103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D6" s="4">
+        <v>44986</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G6" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="7">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="K6" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L6" s="7">
         <v>0</v>
       </c>
       <c r="M6" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N6" s="7">
         <v>0</v>
       </c>
       <c r="O6" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>42103</v>
+        <v>42107</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="4">
-        <v>44986</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="I7" s="7">
-        <v>1000</v>
+        <v>15</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="K7" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L7" s="7">
         <v>0</v>
@@ -907,16 +904,16 @@
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>42107</v>
+        <v>42111</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>16</v>
@@ -941,7 +938,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="7">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M8" s="7">
         <v>0</v>
@@ -951,19 +948,19 @@
       </c>
       <c r="O8" s="7">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>42111</v>
+        <v>42244</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
@@ -975,17 +972,17 @@
         <v>100</v>
       </c>
       <c r="I9" s="7">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" si="0"/>
-        <v>1500</v>
+        <f t="shared" ref="J9:J12" si="2">H9*I9</f>
+        <v>200</v>
       </c>
       <c r="K9" s="7">
         <v>10</v>
       </c>
       <c r="L9" s="7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7">
         <v>0</v>
@@ -994,26 +991,28 @@
         <v>0</v>
       </c>
       <c r="O9" s="7">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="P9" s="4"/>
+        <f t="shared" ref="O9:O12" si="3">K9+L9</f>
+        <v>10</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>42244</v>
+        <v>42278</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H10" s="6">
         <v>100</v>
@@ -1022,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" ref="J10:J13" si="2">H10*I10</f>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="K10" s="7">
@@ -1038,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="7">
-        <f t="shared" ref="O10:O13" si="3">K10+L10</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="P10" s="4" t="s">
@@ -1047,19 +1046,19 @@
     </row>
     <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>42278</v>
+        <v>42326</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="6">
         <v>100</v>
@@ -1093,32 +1092,32 @@
     </row>
     <row r="12" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>42326</v>
+        <v>42359</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H12" s="6">
         <v>100</v>
       </c>
       <c r="I12" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="2"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="K12" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L12" s="7">
         <v>0</v>
@@ -1131,7 +1130,7 @@
       </c>
       <c r="O12" s="7">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P12" s="4" t="s">
         <v>38</v>
@@ -1139,32 +1138,38 @@
     </row>
     <row r="13" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>42359</v>
+        <v>42625</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D13" s="4">
+        <v>49444</v>
+      </c>
+      <c r="E13" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="G13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="6">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="I13" s="7">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="J13:J15" si="4">H13*I13</f>
+        <v>2000</v>
       </c>
       <c r="K13" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L13" s="7">
         <v>0</v>
@@ -1176,47 +1181,39 @@
         <v>0</v>
       </c>
       <c r="O13" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>39</v>
-      </c>
+        <f t="shared" ref="O13:O15" si="5">K13+L13</f>
+        <v>5</v>
+      </c>
+      <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>42625</v>
+        <v>42751</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="4">
-        <v>49444</v>
-      </c>
-      <c r="E14" s="5">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H14" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" ref="J14:J16" si="4">H14*I14</f>
-        <v>2000</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="K14" s="7">
-        <v>5</v>
+        <v>259.8</v>
       </c>
       <c r="L14" s="7">
         <v>0</v>
@@ -1228,24 +1225,30 @@
         <v>0</v>
       </c>
       <c r="O14" s="7">
-        <f t="shared" ref="O14:O16" si="5">K14+L14</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>259.8</v>
       </c>
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>42751</v>
+        <v>42795</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D15" s="4">
+        <v>44986</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G15" s="4" t="s">
         <v>24</v>
       </c>
@@ -1253,17 +1256,17 @@
         <v>1</v>
       </c>
       <c r="I15" s="7">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="J15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="K15" s="7">
-        <v>259.8</v>
+        <v>10</v>
       </c>
       <c r="L15" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M15" s="7">
         <v>0</v>
@@ -1273,47 +1276,41 @@
       </c>
       <c r="O15" s="7">
         <f t="shared" si="5"/>
-        <v>259.8</v>
+        <v>110</v>
       </c>
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>42795</v>
+        <v>42800</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="4">
-        <v>44986</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H16" s="6">
         <v>1</v>
       </c>
       <c r="I16" s="7">
-        <v>850</v>
+        <v>5000</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="4"/>
-        <v>850</v>
+        <f t="shared" ref="J16:J17" si="6">H16*I16</f>
+        <v>5000</v>
       </c>
       <c r="K16" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L16" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M16" s="7">
         <v>0</v>
@@ -1322,42 +1319,48 @@
         <v>0</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="5"/>
-        <v>110</v>
+        <f t="shared" ref="O16:O17" si="7">K16+L16</f>
+        <v>0</v>
       </c>
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>42800</v>
+        <v>43600</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D17" s="4">
+        <v>49444</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="G17" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H17" s="6">
         <v>1</v>
       </c>
       <c r="I17" s="7">
-        <v>5000</v>
+        <v>850</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" ref="J17:J18" si="6">H17*I17</f>
-        <v>5000</v>
+        <f t="shared" si="6"/>
+        <v>850</v>
       </c>
       <c r="K17" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L17" s="7">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="M17" s="7">
         <v>0</v>
@@ -1366,48 +1369,48 @@
         <v>0</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" ref="O17:O18" si="7">K17+L17</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>910</v>
       </c>
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>43600</v>
+        <v>44312</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4">
-        <v>49444</v>
+        <v>45042</v>
       </c>
       <c r="E18" s="5">
-        <v>5.5899999999999998E-2</v>
+        <v>1.5</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H18" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I18" s="7">
         <v>1</v>
       </c>
-      <c r="I18" s="7">
-        <v>850</v>
-      </c>
       <c r="J18" s="7">
-        <f t="shared" si="6"/>
-        <v>850</v>
+        <f t="shared" ref="J18" si="8">H18*I18</f>
+        <v>1000</v>
       </c>
       <c r="K18" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L18" s="7">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="M18" s="7">
         <v>0</v>
@@ -1416,8 +1419,8 @@
         <v>0</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="7"/>
-        <v>910</v>
+        <f t="shared" ref="O18" si="9">K18+L18</f>
+        <v>5</v>
       </c>
       <c r="P18" s="4"/>
     </row>
@@ -1426,19 +1429,19 @@
         <v>44312</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="4">
         <v>45042</v>
       </c>
       <c r="E19" s="5">
-        <v>1.5</v>
+        <v>0.06</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>17</v>
@@ -1450,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="7">
-        <f t="shared" ref="J19:J21" si="8">H19*I19</f>
+        <f t="shared" ref="J19" si="10">H19*I19</f>
         <v>1000</v>
       </c>
       <c r="K19" s="7">
@@ -1466,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="7">
-        <f t="shared" ref="O19:O21" si="9">K19+L19</f>
+        <f t="shared" ref="O19" si="11">K19+L19</f>
         <v>5</v>
       </c>
       <c r="P19" s="4"/>
@@ -1476,19 +1479,19 @@
         <v>44312</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="4">
         <v>45042</v>
       </c>
       <c r="E20" s="5">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>17</v>
@@ -1500,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="7">
-        <f t="shared" ref="J20" si="10">H20*I20</f>
+        <f t="shared" ref="J20:J22" si="12">H20*I20</f>
         <v>1000</v>
       </c>
       <c r="K20" s="7">
@@ -1516,52 +1519,58 @@
         <v>0</v>
       </c>
       <c r="O20" s="7">
-        <f t="shared" ref="O20" si="11">K20+L20</f>
+        <f t="shared" ref="O20:O22" si="13">K20+L20</f>
         <v>5</v>
       </c>
       <c r="P20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>44344</v>
+        <v>44312</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="G21" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H21" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I21" s="7">
         <v>1</v>
       </c>
-      <c r="I21" s="7">
-        <v>0</v>
-      </c>
       <c r="J21" s="7">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>1000</v>
       </c>
       <c r="K21" s="7">
         <v>0</v>
       </c>
       <c r="L21" s="7">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M21" s="7">
         <v>0</v>
       </c>
       <c r="N21" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O21" s="7">
-        <f t="shared" si="9"/>
-        <v>15</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="P21" s="4"/>
     </row>
@@ -1570,22 +1579,22 @@
         <v>44312</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="4">
         <v>45042</v>
       </c>
       <c r="E22" s="5">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H22" s="6">
         <v>1000</v>
@@ -1594,11 +1603,11 @@
         <v>1</v>
       </c>
       <c r="J22" s="7">
-        <f t="shared" ref="J22:J24" si="12">H22*I22</f>
+        <f t="shared" si="12"/>
         <v>1000</v>
       </c>
       <c r="K22" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L22" s="7">
         <v>0</v>
@@ -1610,8 +1619,8 @@
         <v>0</v>
       </c>
       <c r="O22" s="7">
-        <f t="shared" ref="O22:O24" si="13">K22+L22</f>
-        <v>5</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="P22" s="4"/>
     </row>
@@ -1620,22 +1629,22 @@
         <v>44312</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="4">
         <v>45042</v>
       </c>
       <c r="E23" s="5">
-        <v>1.5</v>
+        <v>0.03</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23" s="6">
         <v>1000</v>
@@ -1644,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="J23:J24" si="14">H23*I23</f>
         <v>1000</v>
       </c>
       <c r="K23" s="7">
@@ -1660,42 +1669,36 @@
         <v>0</v>
       </c>
       <c r="O23" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="O23:O24" si="15">K23+L23</f>
         <v>0</v>
       </c>
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>44312</v>
+        <v>41680</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H24" s="6">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="I24" s="7">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="J24" s="7">
-        <f t="shared" si="12"/>
-        <v>1000</v>
+        <f t="shared" si="14"/>
+        <v>6000</v>
       </c>
       <c r="K24" s="7">
         <v>0</v>
@@ -1710,42 +1713,36 @@
         <v>0</v>
       </c>
       <c r="O24" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>44312</v>
+        <v>41708</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H25" s="6">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="I25" s="7">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" ref="J25" si="14">H25*I25</f>
-        <v>1000</v>
+        <f t="shared" ref="J25:J26" si="16">H25*I25</f>
+        <v>7000</v>
       </c>
       <c r="K25" s="7">
         <v>0</v>
@@ -1760,13 +1757,453 @@
         <v>0</v>
       </c>
       <c r="O25" s="7">
-        <f t="shared" ref="O25" si="15">K25+L25</f>
+        <f t="shared" ref="O25:O26" si="17">K25+L25</f>
         <v>0</v>
       </c>
       <c r="P25" s="4"/>
     </row>
+    <row r="26" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>42045</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="6">
+        <v>200</v>
+      </c>
+      <c r="I26" s="7">
+        <v>30</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="16"/>
+        <v>6000</v>
+      </c>
+      <c r="K26" s="7">
+        <v>0</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0</v>
+      </c>
+      <c r="M26" s="7">
+        <v>0</v>
+      </c>
+      <c r="N26" s="7">
+        <v>0</v>
+      </c>
+      <c r="O26" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>42073</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="6">
+        <v>200</v>
+      </c>
+      <c r="I27" s="7">
+        <v>35</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" ref="J27:J28" si="18">H27*I27</f>
+        <v>7000</v>
+      </c>
+      <c r="K27" s="7">
+        <v>0</v>
+      </c>
+      <c r="L27" s="7">
+        <v>0</v>
+      </c>
+      <c r="M27" s="7">
+        <v>0</v>
+      </c>
+      <c r="N27" s="7">
+        <v>0</v>
+      </c>
+      <c r="O27" s="7">
+        <f t="shared" ref="O27:O28" si="19">K27+L27</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>42410</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="6">
+        <v>200</v>
+      </c>
+      <c r="I28" s="7">
+        <v>30</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="18"/>
+        <v>6000</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
+        <v>0</v>
+      </c>
+      <c r="O28" s="7">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>42439</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="6">
+        <v>100</v>
+      </c>
+      <c r="I29" s="7">
+        <v>35</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" ref="J29:J30" si="20">H29*I29</f>
+        <v>3500</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0</v>
+      </c>
+      <c r="L29" s="7">
+        <v>0</v>
+      </c>
+      <c r="M29" s="7">
+        <v>0</v>
+      </c>
+      <c r="N29" s="7">
+        <v>0</v>
+      </c>
+      <c r="O29" s="7">
+        <f t="shared" ref="O29:O30" si="21">K29+L29</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>42470</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="6">
+        <v>200</v>
+      </c>
+      <c r="I30" s="7">
+        <v>30</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" si="20"/>
+        <v>6000</v>
+      </c>
+      <c r="K30" s="7">
+        <v>0</v>
+      </c>
+      <c r="L30" s="7">
+        <v>0</v>
+      </c>
+      <c r="M30" s="7">
+        <v>0</v>
+      </c>
+      <c r="N30" s="7">
+        <v>0</v>
+      </c>
+      <c r="O30" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>42500</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="6">
+        <v>200</v>
+      </c>
+      <c r="I31" s="7">
+        <v>30</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" ref="J31:J35" si="22">H31*I31</f>
+        <v>6000</v>
+      </c>
+      <c r="K31" s="7">
+        <v>0</v>
+      </c>
+      <c r="L31" s="7">
+        <v>0</v>
+      </c>
+      <c r="M31" s="7">
+        <v>0</v>
+      </c>
+      <c r="N31" s="7">
+        <v>0</v>
+      </c>
+      <c r="O31" s="7">
+        <f t="shared" ref="O31:O35" si="23">K31+L31</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>42531</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="6">
+        <v>200</v>
+      </c>
+      <c r="I32" s="7">
+        <v>30</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="22"/>
+        <v>6000</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0</v>
+      </c>
+      <c r="L32" s="7">
+        <v>0</v>
+      </c>
+      <c r="M32" s="7">
+        <v>0</v>
+      </c>
+      <c r="N32" s="7">
+        <v>0</v>
+      </c>
+      <c r="O32" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>42561</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="6">
+        <v>700</v>
+      </c>
+      <c r="I33" s="7">
+        <v>35</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="22"/>
+        <v>24500</v>
+      </c>
+      <c r="K33" s="7">
+        <v>0</v>
+      </c>
+      <c r="L33" s="7">
+        <v>0</v>
+      </c>
+      <c r="M33" s="7">
+        <v>0</v>
+      </c>
+      <c r="N33" s="7">
+        <v>0</v>
+      </c>
+      <c r="O33" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>42695</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="6">
+        <v>100</v>
+      </c>
+      <c r="I34" s="7">
+        <v>5</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="22"/>
+        <v>500</v>
+      </c>
+      <c r="K34" s="7">
+        <v>10</v>
+      </c>
+      <c r="L34" s="7">
+        <v>0</v>
+      </c>
+      <c r="M34" s="7">
+        <v>0</v>
+      </c>
+      <c r="N34" s="7">
+        <v>0</v>
+      </c>
+      <c r="O34" s="7">
+        <f t="shared" si="23"/>
+        <v>10</v>
+      </c>
+      <c r="P34" s="4"/>
+    </row>
+    <row r="35" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>42473</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="6">
+        <v>100</v>
+      </c>
+      <c r="I35" s="7">
+        <v>20</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" si="22"/>
+        <v>2000</v>
+      </c>
+      <c r="K35" s="7">
+        <v>10</v>
+      </c>
+      <c r="L35" s="7">
+        <v>0</v>
+      </c>
+      <c r="M35" s="7">
+        <v>0</v>
+      </c>
+      <c r="N35" s="7">
+        <v>0</v>
+      </c>
+      <c r="O35" s="7">
+        <f t="shared" si="23"/>
+        <v>10</v>
+      </c>
+      <c r="P35" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P25"/>
+  <autoFilter ref="A1:P35"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding CDI benchmark in the summary tab, related to the closed operations results
- Adding CDI benchmark in the summary tab, related to the closed operations results
- Adding some new lines in the PORTFOLIO_TEMPLATE.xlsx file, in order to improve the tests
</commit_message>
<xml_diff>
--- a/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
+++ b/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
   <si>
     <t>Data</t>
   </si>
@@ -564,13 +564,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +633,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>41961</v>
       </c>
@@ -676,9 +677,9 @@
       </c>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>41964</v>
+        <v>36526</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -693,17 +694,17 @@
         <v>17</v>
       </c>
       <c r="H3" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I3" s="7">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="K3" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L3" s="7">
         <v>0</v>
@@ -716,11 +717,11 @@
       </c>
       <c r="O3" s="7">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>41971</v>
       </c>
@@ -770,7 +771,7 @@
       </c>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>42039</v>
       </c>
@@ -814,7 +815,7 @@
       </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>42103</v>
       </c>
@@ -864,9 +865,9 @@
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>42107</v>
+        <v>42095</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
@@ -881,17 +882,17 @@
         <v>17</v>
       </c>
       <c r="H7" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I7" s="7">
-        <v>15</v>
+        <v>2500</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="K7" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L7" s="7">
         <v>0</v>
@@ -904,13 +905,13 @@
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>42111</v>
+        <v>36526</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>18</v>
@@ -925,20 +926,20 @@
         <v>17</v>
       </c>
       <c r="H8" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I8" s="7">
-        <v>15</v>
+        <v>1000</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="K8" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L8" s="7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M8" s="7">
         <v>0</v>
@@ -948,11 +949,11 @@
       </c>
       <c r="O8" s="7">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>42244</v>
       </c>
@@ -998,7 +999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>42278</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>42326</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>42359</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>42625</v>
       </c>
@@ -1186,7 +1187,7 @@
       </c>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>42751</v>
       </c>
@@ -1230,7 +1231,7 @@
       </c>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>42795</v>
       </c>
@@ -1280,7 +1281,7 @@
       </c>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>42800</v>
       </c>
@@ -1324,7 +1325,7 @@
       </c>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43600</v>
       </c>
@@ -1374,7 +1375,7 @@
       </c>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>44312</v>
       </c>
@@ -1424,7 +1425,7 @@
       </c>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>44312</v>
       </c>
@@ -1474,7 +1475,7 @@
       </c>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>44312</v>
       </c>
@@ -1524,9 +1525,9 @@
       </c>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>44312</v>
+        <v>44342</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>30</v>
@@ -1574,9 +1575,9 @@
       </c>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>44312</v>
+        <v>44342</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>30</v>
@@ -1624,9 +1625,9 @@
       </c>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>44312</v>
+        <v>44342</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>30</v>
@@ -1674,7 +1675,7 @@
       </c>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>41680</v>
       </c>
@@ -1718,7 +1719,7 @@
       </c>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>41708</v>
       </c>
@@ -1762,7 +1763,7 @@
       </c>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>42045</v>
       </c>
@@ -1806,7 +1807,7 @@
       </c>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>42073</v>
       </c>
@@ -1850,7 +1851,7 @@
       </c>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>42410</v>
       </c>
@@ -1894,7 +1895,7 @@
       </c>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>42439</v>
       </c>
@@ -1938,7 +1939,7 @@
       </c>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>42470</v>
       </c>
@@ -1982,7 +1983,7 @@
       </c>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>42500</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>30</v>
       </c>
       <c r="J31" s="7">
-        <f t="shared" ref="J31:J35" si="22">H31*I31</f>
+        <f t="shared" ref="J31:J36" si="22">H31*I31</f>
         <v>6000</v>
       </c>
       <c r="K31" s="7">
@@ -2021,12 +2022,12 @@
         <v>0</v>
       </c>
       <c r="O31" s="7">
-        <f t="shared" ref="O31:O35" si="23">K31+L31</f>
+        <f t="shared" ref="O31:O36" si="23">K31+L31</f>
         <v>0</v>
       </c>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>42531</v>
       </c>
@@ -2070,7 +2071,7 @@
       </c>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>42561</v>
       </c>
@@ -2114,9 +2115,9 @@
       </c>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>42695</v>
+        <v>36891</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>15</v>
@@ -2131,17 +2132,17 @@
         <v>24</v>
       </c>
       <c r="H34" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I34" s="7">
-        <v>5</v>
+        <v>1173.19</v>
       </c>
       <c r="J34" s="7">
         <f t="shared" si="22"/>
-        <v>500</v>
+        <v>1173.19</v>
       </c>
       <c r="K34" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L34" s="7">
         <v>0</v>
@@ -2154,13 +2155,13 @@
       </c>
       <c r="O34" s="7">
         <f t="shared" si="23"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>42473</v>
+        <v>42460</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>19</v>
@@ -2175,17 +2176,17 @@
         <v>24</v>
       </c>
       <c r="H35" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I35" s="7">
-        <v>20</v>
+        <v>2843.13</v>
       </c>
       <c r="J35" s="7">
         <f t="shared" si="22"/>
-        <v>2000</v>
+        <v>2843.13</v>
       </c>
       <c r="K35" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L35" s="7">
         <v>0</v>
@@ -2198,12 +2199,67 @@
       </c>
       <c r="O35" s="7">
         <f t="shared" si="23"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P35" s="4"/>
     </row>
+    <row r="36" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>36891</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1</v>
+      </c>
+      <c r="I36" s="7">
+        <v>1059.74</v>
+      </c>
+      <c r="J36" s="7">
+        <f t="shared" si="22"/>
+        <v>1059.74</v>
+      </c>
+      <c r="K36" s="7">
+        <v>0</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0</v>
+      </c>
+      <c r="M36" s="7">
+        <v>0</v>
+      </c>
+      <c r="N36" s="7">
+        <v>0</v>
+      </c>
+      <c r="O36" s="7">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P35"/>
+  <autoFilter ref="A1:P35">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="CIEL3"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Ações"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Adding CDI benchmark in the summary tab, related to the closed operations results"
This reverts commit 448e4aa123365e78dbbda0c62a0cce152f0890fb.
</commit_message>
<xml_diff>
--- a/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
+++ b/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="43">
   <si>
     <t>Data</t>
   </si>
@@ -564,14 +564,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +632,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>41961</v>
       </c>
@@ -677,9 +676,9 @@
       </c>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>36526</v>
+        <v>41964</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -694,17 +693,17 @@
         <v>17</v>
       </c>
       <c r="H3" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I3" s="7">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="K3" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L3" s="7">
         <v>0</v>
@@ -717,11 +716,11 @@
       </c>
       <c r="O3" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>41971</v>
       </c>
@@ -771,7 +770,7 @@
       </c>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>42039</v>
       </c>
@@ -815,7 +814,7 @@
       </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>42103</v>
       </c>
@@ -865,9 +864,9 @@
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>42095</v>
+        <v>42107</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
@@ -882,17 +881,17 @@
         <v>17</v>
       </c>
       <c r="H7" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I7" s="7">
-        <v>2500</v>
+        <v>15</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="K7" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L7" s="7">
         <v>0</v>
@@ -905,13 +904,13 @@
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>36526</v>
+        <v>42111</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>18</v>
@@ -926,20 +925,20 @@
         <v>17</v>
       </c>
       <c r="H8" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I8" s="7">
-        <v>1000</v>
+        <v>15</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K8" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L8" s="7">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M8" s="7">
         <v>0</v>
@@ -949,11 +948,11 @@
       </c>
       <c r="O8" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>42244</v>
       </c>
@@ -999,7 +998,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>42278</v>
       </c>
@@ -1045,7 +1044,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>42326</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>42359</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>42625</v>
       </c>
@@ -1187,7 +1186,7 @@
       </c>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>42751</v>
       </c>
@@ -1231,7 +1230,7 @@
       </c>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>42795</v>
       </c>
@@ -1281,7 +1280,7 @@
       </c>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>42800</v>
       </c>
@@ -1325,7 +1324,7 @@
       </c>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43600</v>
       </c>
@@ -1375,7 +1374,7 @@
       </c>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>44312</v>
       </c>
@@ -1425,7 +1424,7 @@
       </c>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>44312</v>
       </c>
@@ -1475,7 +1474,7 @@
       </c>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>44312</v>
       </c>
@@ -1525,9 +1524,9 @@
       </c>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>44342</v>
+        <v>44312</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>30</v>
@@ -1575,9 +1574,9 @@
       </c>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>44342</v>
+        <v>44312</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>30</v>
@@ -1625,9 +1624,9 @@
       </c>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>44342</v>
+        <v>44312</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>30</v>
@@ -1675,7 +1674,7 @@
       </c>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>41680</v>
       </c>
@@ -1719,7 +1718,7 @@
       </c>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>41708</v>
       </c>
@@ -1763,7 +1762,7 @@
       </c>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>42045</v>
       </c>
@@ -1807,7 +1806,7 @@
       </c>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>42073</v>
       </c>
@@ -1851,7 +1850,7 @@
       </c>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>42410</v>
       </c>
@@ -1895,7 +1894,7 @@
       </c>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>42439</v>
       </c>
@@ -1939,7 +1938,7 @@
       </c>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>42470</v>
       </c>
@@ -1983,7 +1982,7 @@
       </c>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>42500</v>
       </c>
@@ -2006,7 +2005,7 @@
         <v>30</v>
       </c>
       <c r="J31" s="7">
-        <f t="shared" ref="J31:J36" si="22">H31*I31</f>
+        <f t="shared" ref="J31:J35" si="22">H31*I31</f>
         <v>6000</v>
       </c>
       <c r="K31" s="7">
@@ -2022,12 +2021,12 @@
         <v>0</v>
       </c>
       <c r="O31" s="7">
-        <f t="shared" ref="O31:O36" si="23">K31+L31</f>
+        <f t="shared" ref="O31:O35" si="23">K31+L31</f>
         <v>0</v>
       </c>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>42531</v>
       </c>
@@ -2071,7 +2070,7 @@
       </c>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>42561</v>
       </c>
@@ -2115,9 +2114,9 @@
       </c>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>36891</v>
+        <v>42695</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>15</v>
@@ -2132,17 +2131,17 @@
         <v>24</v>
       </c>
       <c r="H34" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I34" s="7">
-        <v>1173.19</v>
+        <v>5</v>
       </c>
       <c r="J34" s="7">
         <f t="shared" si="22"/>
-        <v>1173.19</v>
+        <v>500</v>
       </c>
       <c r="K34" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L34" s="7">
         <v>0</v>
@@ -2155,13 +2154,13 @@
       </c>
       <c r="O34" s="7">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>42460</v>
+        <v>42473</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>19</v>
@@ -2176,17 +2175,17 @@
         <v>24</v>
       </c>
       <c r="H35" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I35" s="7">
-        <v>2843.13</v>
+        <v>20</v>
       </c>
       <c r="J35" s="7">
         <f t="shared" si="22"/>
-        <v>2843.13</v>
+        <v>2000</v>
       </c>
       <c r="K35" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L35" s="7">
         <v>0</v>
@@ -2199,67 +2198,12 @@
       </c>
       <c r="O35" s="7">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>36891</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="6">
-        <v>1</v>
-      </c>
-      <c r="I36" s="7">
-        <v>1059.74</v>
-      </c>
-      <c r="J36" s="7">
-        <f t="shared" si="22"/>
-        <v>1059.74</v>
-      </c>
-      <c r="K36" s="7">
-        <v>0</v>
-      </c>
-      <c r="L36" s="7">
-        <v>0</v>
-      </c>
-      <c r="M36" s="7">
-        <v>0</v>
-      </c>
-      <c r="N36" s="7">
-        <v>0</v>
-      </c>
-      <c r="O36" s="7">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="P36" s="4"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P35">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="CIEL3"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Ações"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P35"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Solving some issues related to empty Extrato Excel files
- Solved some issues related to empty Extrato Excel files
- Changed the column name from 'Rentabilidade Contratada' to 'Rentabilidade-média Contratada'
- Updated the Excel portfolio template files
- Some other changes with small end-user impact
</commit_message>
<xml_diff>
--- a/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
+++ b/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="45">
   <si>
     <t>Data</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Resgate</t>
   </si>
   <si>
-    <t>LC (SANTANA CFI) - 26/ABR/2023</t>
-  </si>
-  <si>
     <t>CDI</t>
   </si>
   <si>
@@ -169,6 +166,15 @@
   </si>
   <si>
     <t>Tesouro IPCA+ 2035</t>
+  </si>
+  <si>
+    <t>LC (SANTANA CDI) - 26/ABR/2023</t>
+  </si>
+  <si>
+    <t>LC (SANTANA IPCA) - 26/ABR/2023</t>
+  </si>
+  <si>
+    <t>LC (SANTANA PREFIXADO) - 26/ABR/2023</t>
   </si>
 </sst>
 </file>
@@ -567,10 +573,10 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,16 +626,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -725,10 +731,10 @@
         <v>41971</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4">
         <v>49444</v>
@@ -819,10 +825,10 @@
         <v>42103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="4">
         <v>44986</v>
@@ -995,7 +1001,7 @@
         <v>10</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1041,7 +1047,7 @@
         <v>10</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1087,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1133,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1141,10 +1147,10 @@
         <v>42625</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4">
         <v>49444</v>
@@ -1191,10 +1197,10 @@
         <v>42751</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
@@ -1235,10 +1241,10 @@
         <v>42795</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4">
         <v>44986</v>
@@ -1329,10 +1335,10 @@
         <v>43600</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4">
         <v>49444</v>
@@ -1379,10 +1385,10 @@
         <v>44312</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="4">
         <v>45042</v>
@@ -1391,7 +1397,7 @@
         <v>1.5</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>17</v>
@@ -1424,15 +1430,15 @@
       </c>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>44312</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="4">
         <v>45042</v>
@@ -1479,10 +1485,10 @@
         <v>44312</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="4">
         <v>45042</v>
@@ -1529,10 +1535,10 @@
         <v>44312</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="4">
         <v>45042</v>
@@ -1541,7 +1547,7 @@
         <v>1.5</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>24</v>
@@ -1574,15 +1580,15 @@
       </c>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>44312</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="4">
         <v>45042</v>
@@ -1629,10 +1635,10 @@
         <v>44312</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="4">
         <v>45042</v>

</xml_diff>

<commit_message>
Solving the issue (#65) related to the 'portfolio_investment.py' running alone
- Adding some try/except statements to solve the mentioned main issue
- Printing the current 'Renda Variável', 'Renda Fixa' and 'Tesouro Direto' dataframes
- Replacing the directory manipulation to use the 'os.path.join' method
</commit_message>
<xml_diff>
--- a/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
+++ b/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Extrato" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$P$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$P$34</definedName>
     <definedName name="Aplica">#REF!</definedName>
     <definedName name="CDI">#REF!</definedName>
     <definedName name="IR0.0">#REF!</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="45">
   <si>
     <t>Data</t>
   </si>
@@ -570,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2011,7 +2011,7 @@
         <v>30</v>
       </c>
       <c r="J31" s="7">
-        <f t="shared" ref="J31:J35" si="22">H31*I31</f>
+        <f t="shared" ref="J31:J34" si="22">H31*I31</f>
         <v>6000</v>
       </c>
       <c r="K31" s="7">
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="O31" s="7">
-        <f t="shared" ref="O31:O35" si="23">K31+L31</f>
+        <f t="shared" ref="O31:O34" si="23">K31+L31</f>
         <v>0</v>
       </c>
       <c r="P31" s="4"/>
@@ -2164,52 +2164,8 @@
       </c>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>42473</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" s="6">
-        <v>100</v>
-      </c>
-      <c r="I35" s="7">
-        <v>20</v>
-      </c>
-      <c r="J35" s="7">
-        <f t="shared" si="22"/>
-        <v>2000</v>
-      </c>
-      <c r="K35" s="7">
-        <v>10</v>
-      </c>
-      <c r="L35" s="7">
-        <v>0</v>
-      </c>
-      <c r="M35" s="7">
-        <v>0</v>
-      </c>
-      <c r="N35" s="7">
-        <v>0</v>
-      </c>
-      <c r="O35" s="7">
-        <f t="shared" si="23"/>
-        <v>10</v>
-      </c>
-      <c r="P35" s="4"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P35"/>
+  <autoFilter ref="A1:P34"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Additional refactoring in 'portfolio_investment.py' file
- Created the files:
   > portfolio_investment_test.py
   >  portfolio_statistics.py (unuseful methods from 'PortfolioInvestment' class)
- Updated the 'VariableIncome' class with some other methods from 'PortfolioInvestment' class
- Some other changes with small impact
</commit_message>
<xml_diff>
--- a/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
+++ b/portfolio_lib/PORTFOLIO_TEMPLATE.xlsx
@@ -573,10 +573,10 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,14 +1403,14 @@
         <v>17</v>
       </c>
       <c r="H18" s="6">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="I18" s="7">
         <v>1</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" ref="J18" si="8">H18*I18</f>
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="K18" s="7">
         <v>5</v>
@@ -1453,14 +1453,14 @@
         <v>17</v>
       </c>
       <c r="H19" s="6">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="I19" s="7">
         <v>1</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" ref="J19" si="10">H19*I19</f>
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="K19" s="7">
         <v>5</v>
@@ -1503,14 +1503,14 @@
         <v>17</v>
       </c>
       <c r="H20" s="6">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="I20" s="7">
         <v>1</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" ref="J20:J22" si="12">H20*I20</f>
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="K20" s="7">
         <v>5</v>

</xml_diff>